<commit_message>
CIR-1787-Updated XLS/CVS service guide for story
</commit_message>
<xml_diff>
--- a/source/downloads/business-rules/Full Return Business Rules.xlsx
+++ b/source/downloads/business-rules/Full Return Business Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamcooper/Documents/GitHub/irr-api-end-to-end-service-guide/source/downloads/business-rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9153753C-0E4C-684F-BF3F-1F3C8A7B3AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B184A09E-29A1-F74E-A08C-78068A39906D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="37020" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7040" yWindow="460" windowWidth="31360" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Return Business Rules" sheetId="1" r:id="rId1"/>
@@ -345,19 +345,6 @@
 min 0%, max 100%
 5 decimal places.
 No rounding up or down of the figure</t>
-  </si>
-  <si>
-    <t>Only required where a groupRatio isElected  = True
-Cannot be a negative value
-The group ratio percentage is capped at 100%
-The ratio % will = 100% if the calculation gives a negative result 
-When EBITDA = zero, Group ratio will = 100% 
-When QNGIE = zero, Group ratio will = 0%
-An Error message will be returned if data is not provided
-Examples:
-QNGIE divided by EBITDA gives a negative value, then Group ratio = 100%?
-When EBITDA that is zero, the Group ratio is = 100%??
-QNGIE divided by EBITDA = 120%, then Group ratio = 100%</t>
   </si>
   <si>
     <t>(groupRatioBlended)
@@ -713,6 +700,20 @@
   <si>
     <t>A company can have a net tax - interest expense and a reactivation</t>
   </si>
+  <si>
+    <t>Only required where a groupRatio isElected  = True
+Cannot be a negative value
+The group ratio percentage is capped at 100%
+The ratio % will = 100% if the calculation gives a negative result 
+When EBITDA = zero, Group ratio will = 100% 
+When QNGIE = zero, Group ratio will = 0%
+An Error message will be returned if data is not provided
+Where a Group ratio (blended) election is made, the calculation of the group ratio percentage is different. It still cannot be a negative number and is still capped at 100%.
+Examples:
+QNGIE divided by EBITDA gives a negative value, then Group ratio = 100%?
+When EBITDA that is zero, the Group ratio is = 100%??
+QNGIE divided by EBITDA = 120%, then Group ratio = 100%</t>
+  </si>
 </sst>
 </file>
 
@@ -1043,12 +1044,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1058,17 +1070,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1292,8 +1293,8 @@
   <dimension ref="A1:T884"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1339,15 +1340,15 @@
       <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" ht="13">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="49"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1376,7 +1377,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="8"/>
@@ -1459,13 +1460,13 @@
       <c r="T5" s="3"/>
     </row>
     <row r="6" spans="1:20" ht="13">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="20"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
@@ -1547,13 +1548,13 @@
       <c r="T8" s="3"/>
     </row>
     <row r="9" spans="1:20" ht="13">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="41"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
@@ -1603,12 +1604,12 @@
       <c r="T10" s="3"/>
     </row>
     <row r="11" spans="1:20" ht="126">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1629,13 +1630,13 @@
       <c r="T11" s="3"/>
     </row>
     <row r="12" spans="1:20" ht="13">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="41"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="20"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
@@ -1749,13 +1750,13 @@
       <c r="T15" s="3"/>
     </row>
     <row r="16" spans="1:20" ht="13">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="41"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
       <c r="F16" s="20"/>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
@@ -1869,13 +1870,13 @@
       <c r="T19" s="3"/>
     </row>
     <row r="20" spans="1:20" ht="13">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="41"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
@@ -2337,13 +2338,13 @@
       <c r="T34" s="3"/>
     </row>
     <row r="35" spans="1:20" ht="13">
-      <c r="A35" s="47" t="s">
+      <c r="A35" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="41"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="39"/>
       <c r="F35" s="20"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -2456,7 +2457,7 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20" ht="154">
+    <row r="39" spans="1:20" ht="196">
       <c r="A39" s="4">
         <v>5.4</v>
       </c>
@@ -2470,7 +2471,7 @@
         <v>79</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
       <c r="F39" s="20"/>
       <c r="G39" s="8"/>
@@ -2493,7 +2494,7 @@
         <v>5.5</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>7</v>
@@ -2502,7 +2503,7 @@
         <v>8</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F40" s="20"/>
       <c r="G40" s="8"/>
@@ -2525,16 +2526,16 @@
         <v>5.6</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F41" s="20"/>
       <c r="G41" s="8"/>
@@ -2554,10 +2555,10 @@
     </row>
     <row r="42" spans="1:20" ht="28">
       <c r="A42" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>7</v>
@@ -2566,7 +2567,7 @@
         <v>8</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F42" s="23"/>
       <c r="G42" s="3"/>
@@ -2589,7 +2590,7 @@
         <v>5.7</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>7</v>
@@ -2598,7 +2599,7 @@
         <v>8</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F43" s="20"/>
       <c r="G43" s="3"/>
@@ -2617,13 +2618,13 @@
       <c r="T43" s="3"/>
     </row>
     <row r="44" spans="1:20" ht="13">
-      <c r="A44" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="41"/>
+      <c r="A44" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="39"/>
       <c r="F44" s="20"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -2645,16 +2646,16 @@
         <v>5.8</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="D45" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="E45" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F45" s="23"/>
       <c r="G45" s="8"/>
@@ -2677,7 +2678,7 @@
         <v>5.9</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>7</v>
@@ -2686,7 +2687,7 @@
         <v>8</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="3"/>
@@ -2706,10 +2707,10 @@
     </row>
     <row r="47" spans="1:20" ht="28">
       <c r="A47" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>7</v>
@@ -2718,7 +2719,7 @@
         <v>8</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="3"/>
@@ -2738,10 +2739,10 @@
     </row>
     <row r="48" spans="1:20" ht="98">
       <c r="A48" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>7</v>
@@ -2750,7 +2751,7 @@
         <v>8</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F48" s="26"/>
       <c r="G48" s="8"/>
@@ -2773,7 +2774,7 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>7</v>
@@ -2782,7 +2783,7 @@
         <v>8</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F49" s="20"/>
       <c r="G49" s="8"/>
@@ -2802,10 +2803,10 @@
     </row>
     <row r="50" spans="1:20" ht="42">
       <c r="A50" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>7</v>
@@ -2814,7 +2815,7 @@
         <v>8</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F50" s="20"/>
       <c r="G50" s="3"/>
@@ -2837,7 +2838,7 @@
         <v>5.12</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>7</v>
@@ -2846,7 +2847,7 @@
         <v>8</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="3"/>
@@ -2865,13 +2866,13 @@
       <c r="T51" s="3"/>
     </row>
     <row r="52" spans="1:20" ht="13">
-      <c r="A52" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="B52" s="40"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="41"/>
+      <c r="A52" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="39"/>
       <c r="F52" s="20"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -2893,16 +2894,16 @@
         <v>5.13</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="D53" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="8"/>
@@ -2921,13 +2922,13 @@
       <c r="T53" s="3"/>
     </row>
     <row r="54" spans="1:20" ht="13">
-      <c r="A54" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="B54" s="40"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="41"/>
+      <c r="A54" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="39"/>
       <c r="F54" s="20"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -2949,16 +2950,16 @@
         <v>5.14</v>
       </c>
       <c r="B55" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="D55" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="F55" s="20"/>
       <c r="G55" s="8"/>
@@ -2981,7 +2982,7 @@
         <v>5.15</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>19</v>
@@ -3007,13 +3008,13 @@
       <c r="T56" s="3"/>
     </row>
     <row r="57" spans="1:20" ht="13">
-      <c r="A57" s="46" t="s">
-        <v>126</v>
-      </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="41"/>
+      <c r="A57" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="39"/>
       <c r="F57" s="20"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -3031,13 +3032,13 @@
       <c r="T57" s="3"/>
     </row>
     <row r="58" spans="1:20" ht="13">
-      <c r="A58" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="41"/>
+      <c r="A58" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="39"/>
       <c r="F58" s="20"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -3062,7 +3063,7 @@
         <v>16</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>8</v>
@@ -3091,7 +3092,7 @@
         <v>6.2</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>19</v>
@@ -3123,7 +3124,7 @@
         <v>6.3</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>7</v>
@@ -3155,16 +3156,16 @@
         <v>6.4</v>
       </c>
       <c r="B62" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="D62" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="D62" s="29" t="s">
-        <v>133</v>
-      </c>
       <c r="E62" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F62" s="20"/>
       <c r="G62" s="3"/>
@@ -3187,16 +3188,16 @@
         <v>6.5</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D63" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="C63" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D63" s="29" t="s">
+      <c r="E63" s="30" t="s">
         <v>135</v>
-      </c>
-      <c r="E63" s="30" t="s">
-        <v>136</v>
       </c>
       <c r="F63" s="20"/>
       <c r="G63" s="3"/>
@@ -3219,7 +3220,7 @@
         <v>6.6</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>82</v>
@@ -3228,7 +3229,7 @@
         <v>8</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F64" s="20"/>
       <c r="G64" s="3"/>
@@ -3251,14 +3252,14 @@
         <v>6.7</v>
       </c>
       <c r="B65" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>140</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F65" s="20"/>
       <c r="G65" s="8"/>
@@ -3281,14 +3282,14 @@
         <v>6.9</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F66" s="20"/>
       <c r="G66" s="8"/>
@@ -3307,20 +3308,20 @@
       <c r="T66" s="3"/>
     </row>
     <row r="67" spans="1:20" ht="42">
-      <c r="A67" s="42">
+      <c r="A67" s="47">
         <v>6.1</v>
       </c>
       <c r="B67" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="D67" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="33" t="s">
         <v>144</v>
-      </c>
-      <c r="D67" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="33" t="s">
-        <v>145</v>
       </c>
       <c r="F67" s="20"/>
       <c r="G67" s="8"/>
@@ -3339,14 +3340,14 @@
       <c r="T67" s="3"/>
     </row>
     <row r="68" spans="1:20" ht="14">
-      <c r="A68" s="43"/>
+      <c r="A68" s="48"/>
       <c r="B68" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D68" s="43"/>
+      <c r="D68" s="48"/>
       <c r="E68" s="33"/>
       <c r="F68" s="20"/>
       <c r="G68" s="3"/>
@@ -3365,20 +3366,20 @@
       <c r="T68" s="3"/>
     </row>
     <row r="69" spans="1:20" ht="42">
-      <c r="A69" s="42">
+      <c r="A69" s="47">
         <v>6.11</v>
       </c>
       <c r="B69" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C69" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D69" s="45" t="s">
+      <c r="D69" s="50" t="s">
         <v>41</v>
       </c>
       <c r="E69" s="34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F69" s="20"/>
       <c r="G69" s="3"/>
@@ -3397,14 +3398,14 @@
       <c r="T69" s="3"/>
     </row>
     <row r="70" spans="1:20" ht="14">
-      <c r="A70" s="43"/>
+      <c r="A70" s="48"/>
       <c r="B70" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C70" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D70" s="43"/>
+      <c r="D70" s="48"/>
       <c r="E70" s="35"/>
       <c r="F70" s="20"/>
       <c r="G70" s="3"/>
@@ -3423,20 +3424,20 @@
       <c r="T70" s="3"/>
     </row>
     <row r="71" spans="1:20" ht="56">
-      <c r="A71" s="42">
+      <c r="A71" s="47">
         <v>6.12</v>
       </c>
       <c r="B71" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C71" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="D71" s="45" t="s">
+      <c r="D71" s="50" t="s">
         <v>41</v>
       </c>
       <c r="E71" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F71" s="20"/>
       <c r="G71" s="3"/>
@@ -3455,14 +3456,14 @@
       <c r="T71" s="3"/>
     </row>
     <row r="72" spans="1:20" ht="14">
-      <c r="A72" s="43"/>
+      <c r="A72" s="48"/>
       <c r="B72" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C72" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D72" s="43"/>
+      <c r="D72" s="48"/>
       <c r="E72" s="35"/>
       <c r="F72" s="20"/>
       <c r="G72" s="3"/>
@@ -3485,14 +3486,14 @@
         <v>6.13</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>68</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F73" s="27"/>
       <c r="G73" s="8"/>
@@ -3511,13 +3512,13 @@
       <c r="T73" s="3"/>
     </row>
     <row r="74" spans="1:20" ht="13">
-      <c r="A74" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="B74" s="40"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="40"/>
-      <c r="E74" s="41"/>
+      <c r="A74" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="B74" s="38"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="39"/>
       <c r="F74" s="20"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
@@ -3535,10 +3536,10 @@
       <c r="T74" s="3"/>
     </row>
     <row r="75" spans="1:20" ht="13">
-      <c r="A75" s="36"/>
-      <c r="B75" s="37"/>
-      <c r="C75" s="37"/>
-      <c r="D75" s="38"/>
+      <c r="A75" s="42"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="44"/>
       <c r="E75" s="13"/>
       <c r="F75" s="20"/>
       <c r="G75" s="3"/>
@@ -3561,7 +3562,7 @@
         <v>6.14</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>68</v>
@@ -3569,8 +3570,8 @@
       <c r="D76" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E76" s="50" t="s">
-        <v>173</v>
+      <c r="E76" s="36" t="s">
+        <v>172</v>
       </c>
       <c r="F76" s="20"/>
       <c r="G76" s="8"/>
@@ -3593,14 +3594,14 @@
         <v>6.15</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F77" s="20"/>
       <c r="G77" s="3"/>
@@ -3620,16 +3621,16 @@
     </row>
     <row r="78" spans="1:20" ht="42">
       <c r="A78" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B78" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>10</v>
@@ -3655,7 +3656,7 @@
         <v>7.1</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>7</v>
@@ -3664,7 +3665,7 @@
         <v>8</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F79" s="20"/>
       <c r="G79" s="3"/>
@@ -21394,21 +21395,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A54:E54"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A74:E74"/>
     <mergeCell ref="A75:D75"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A67:A68"/>
@@ -21417,6 +21403,21 @@
     <mergeCell ref="D69:D70"/>
     <mergeCell ref="A71:A72"/>
     <mergeCell ref="D71:D72"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A74:E74"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CIR-1825 updated buisness rules csv & xlsx
</commit_message>
<xml_diff>
--- a/source/downloads/business-rules/Full Return Business Rules.xlsx
+++ b/source/downloads/business-rules/Full Return Business Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamcooper/Documents/GitHub/irr-api-end-to-end-service-guide/source/downloads/business-rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B184A09E-29A1-F74E-A08C-78068A39906D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F675F72-18D1-5449-A04F-0F363EC0F9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="460" windowWidth="31360" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="460" windowWidth="27640" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Return Business Rules" sheetId="1" r:id="rId1"/>
@@ -319,23 +319,11 @@
     <t>M if 5.1 = Yes</t>
   </si>
   <si>
-    <t>Qualifying net group-interest expense (QNGIE)
-Only required where groupRatio isElected  = True
-An Error message will be returned if data is not provided and 5.1 = True</t>
-  </si>
-  <si>
     <t>groupEBITDA</t>
   </si>
   <si>
     <t>Numeric
 no-min, no-max</t>
-  </si>
-  <si>
-    <t>Group-EBITDA
-(Earnings Before Interest, Taxes, Depreciation and Amortisation)
-Only required where a groupRatio isElected  = True
-An Error message will be returned if data is not provided and 5.1 = True
-Group-EBITDA can be a negative amount.</t>
   </si>
   <si>
     <t>groupRatio</t>
@@ -714,6 +702,20 @@
 When EBITDA that is zero, the Group ratio is = 100%??
 QNGIE divided by EBITDA = 120%, then Group ratio = 100%</t>
   </si>
+  <si>
+    <t>Qualifying net group-interest expense (QNGIE)
+Only required where groupRatio isElected  = True
+An Error message will be returned if data is not provided and 5.1 = True
+Where a Group Ratio (Blended) Election is made, this field should be populated with the figure of blended net group-interest expense.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group-EBITDA
+(Earnings Before Interest, Taxes, Depreciation and Amortisation)
+Only required where a groupRatio isElected  = True &amp; groupRatioBlended = False
+An Error message will be returned if data is not provided and 5.1 = True &amp; 5.5 = False
+Group-EBITDA can be a negative amount.
+Note this field is not required when a Group Ratio (Blended) Election is made. </t>
+  </si>
 </sst>
 </file>
 
@@ -961,7 +963,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1047,20 +1049,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1070,6 +1064,17 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1293,8 +1298,8 @@
   <dimension ref="A1:T884"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1340,15 +1345,15 @@
       <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" ht="13">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1377,7 +1382,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="8"/>
@@ -1460,13 +1465,13 @@
       <c r="T5" s="3"/>
     </row>
     <row r="6" spans="1:20" ht="13">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="20"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
@@ -1548,13 +1553,13 @@
       <c r="T8" s="3"/>
     </row>
     <row r="9" spans="1:20" ht="13">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="39"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
@@ -1604,12 +1609,12 @@
       <c r="T10" s="3"/>
     </row>
     <row r="11" spans="1:20" ht="126">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
       <c r="E11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1630,13 +1635,13 @@
       <c r="T11" s="3"/>
     </row>
     <row r="12" spans="1:20" ht="13">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="20"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
@@ -1750,13 +1755,13 @@
       <c r="T15" s="3"/>
     </row>
     <row r="16" spans="1:20" ht="13">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="20"/>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
@@ -1870,13 +1875,13 @@
       <c r="T19" s="3"/>
     </row>
     <row r="20" spans="1:20" ht="13">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
@@ -2338,13 +2343,13 @@
       <c r="T34" s="3"/>
     </row>
     <row r="35" spans="1:20" ht="13">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="39"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42"/>
       <c r="F35" s="20"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -2393,7 +2398,7 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20" ht="42">
+    <row r="37" spans="1:20" ht="78" customHeight="1">
       <c r="A37" s="4">
         <v>5.2</v>
       </c>
@@ -2406,8 +2411,8 @@
       <c r="D37" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>80</v>
+      <c r="E37" s="51" t="s">
+        <v>172</v>
       </c>
       <c r="F37" s="20"/>
       <c r="G37" s="3"/>
@@ -2425,21 +2430,21 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20" ht="70">
+    <row r="38" spans="1:20" ht="98" customHeight="1">
       <c r="A38" s="4">
         <v>5.3</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>83</v>
+      <c r="E38" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="F38" s="20"/>
       <c r="G38" s="8"/>
@@ -2462,16 +2467,16 @@
         <v>5.4</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>79</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F39" s="20"/>
       <c r="G39" s="8"/>
@@ -2494,7 +2499,7 @@
         <v>5.5</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>7</v>
@@ -2503,7 +2508,7 @@
         <v>8</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F40" s="20"/>
       <c r="G40" s="8"/>
@@ -2526,16 +2531,16 @@
         <v>5.6</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F41" s="20"/>
       <c r="G41" s="8"/>
@@ -2555,10 +2560,10 @@
     </row>
     <row r="42" spans="1:20" ht="28">
       <c r="A42" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>7</v>
@@ -2567,7 +2572,7 @@
         <v>8</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F42" s="23"/>
       <c r="G42" s="3"/>
@@ -2590,7 +2595,7 @@
         <v>5.7</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>7</v>
@@ -2599,7 +2604,7 @@
         <v>8</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F43" s="20"/>
       <c r="G43" s="3"/>
@@ -2618,13 +2623,13 @@
       <c r="T43" s="3"/>
     </row>
     <row r="44" spans="1:20" ht="13">
-      <c r="A44" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="39"/>
+      <c r="A44" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="42"/>
       <c r="F44" s="20"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -2646,16 +2651,16 @@
         <v>5.8</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="E45" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F45" s="23"/>
       <c r="G45" s="8"/>
@@ -2678,7 +2683,7 @@
         <v>5.9</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>7</v>
@@ -2687,7 +2692,7 @@
         <v>8</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="3"/>
@@ -2707,10 +2712,10 @@
     </row>
     <row r="47" spans="1:20" ht="28">
       <c r="A47" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>7</v>
@@ -2719,7 +2724,7 @@
         <v>8</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="3"/>
@@ -2739,10 +2744,10 @@
     </row>
     <row r="48" spans="1:20" ht="98">
       <c r="A48" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>7</v>
@@ -2751,7 +2756,7 @@
         <v>8</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F48" s="26"/>
       <c r="G48" s="8"/>
@@ -2774,7 +2779,7 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>7</v>
@@ -2783,7 +2788,7 @@
         <v>8</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F49" s="20"/>
       <c r="G49" s="8"/>
@@ -2803,10 +2808,10 @@
     </row>
     <row r="50" spans="1:20" ht="42">
       <c r="A50" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>7</v>
@@ -2815,7 +2820,7 @@
         <v>8</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F50" s="20"/>
       <c r="G50" s="3"/>
@@ -2838,7 +2843,7 @@
         <v>5.12</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>7</v>
@@ -2847,7 +2852,7 @@
         <v>8</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="3"/>
@@ -2866,13 +2871,13 @@
       <c r="T51" s="3"/>
     </row>
     <row r="52" spans="1:20" ht="13">
-      <c r="A52" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="39"/>
+      <c r="A52" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" s="41"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="42"/>
       <c r="F52" s="20"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -2894,16 +2899,16 @@
         <v>5.13</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="E53" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="8"/>
@@ -2922,13 +2927,13 @@
       <c r="T53" s="3"/>
     </row>
     <row r="54" spans="1:20" ht="13">
-      <c r="A54" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="B54" s="38"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="39"/>
+      <c r="A54" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54" s="41"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="42"/>
       <c r="F54" s="20"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -2950,16 +2955,16 @@
         <v>5.14</v>
       </c>
       <c r="B55" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="E55" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="F55" s="20"/>
       <c r="G55" s="8"/>
@@ -2982,7 +2987,7 @@
         <v>5.15</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>19</v>
@@ -3008,13 +3013,13 @@
       <c r="T56" s="3"/>
     </row>
     <row r="57" spans="1:20" ht="13">
-      <c r="A57" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="B57" s="38"/>
-      <c r="C57" s="38"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="39"/>
+      <c r="A57" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" s="41"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="41"/>
+      <c r="E57" s="42"/>
       <c r="F57" s="20"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -3032,13 +3037,13 @@
       <c r="T57" s="3"/>
     </row>
     <row r="58" spans="1:20" ht="13">
-      <c r="A58" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="B58" s="38"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="39"/>
+      <c r="A58" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B58" s="41"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="41"/>
+      <c r="E58" s="42"/>
       <c r="F58" s="20"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -3063,7 +3068,7 @@
         <v>16</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>8</v>
@@ -3092,7 +3097,7 @@
         <v>6.2</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>19</v>
@@ -3124,7 +3129,7 @@
         <v>6.3</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>7</v>
@@ -3156,16 +3161,16 @@
         <v>6.4</v>
       </c>
       <c r="B62" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="C62" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D62" s="29" t="s">
-        <v>132</v>
-      </c>
       <c r="E62" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F62" s="20"/>
       <c r="G62" s="3"/>
@@ -3188,16 +3193,16 @@
         <v>6.5</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="E63" s="30" t="s">
         <v>133</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="E63" s="30" t="s">
-        <v>135</v>
       </c>
       <c r="F63" s="20"/>
       <c r="G63" s="3"/>
@@ -3220,16 +3225,16 @@
         <v>6.6</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D64" s="29" t="s">
         <v>8</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F64" s="20"/>
       <c r="G64" s="3"/>
@@ -3252,14 +3257,14 @@
         <v>6.7</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F65" s="20"/>
       <c r="G65" s="8"/>
@@ -3282,14 +3287,14 @@
         <v>6.9</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F66" s="20"/>
       <c r="G66" s="8"/>
@@ -3308,20 +3313,20 @@
       <c r="T66" s="3"/>
     </row>
     <row r="67" spans="1:20" ht="42">
-      <c r="A67" s="47">
+      <c r="A67" s="43">
         <v>6.1</v>
       </c>
       <c r="B67" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D67" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="33" t="s">
         <v>142</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D67" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="33" t="s">
-        <v>144</v>
       </c>
       <c r="F67" s="20"/>
       <c r="G67" s="8"/>
@@ -3340,14 +3345,14 @@
       <c r="T67" s="3"/>
     </row>
     <row r="68" spans="1:20" ht="14">
-      <c r="A68" s="48"/>
+      <c r="A68" s="44"/>
       <c r="B68" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D68" s="48"/>
+        <v>144</v>
+      </c>
+      <c r="D68" s="44"/>
       <c r="E68" s="33"/>
       <c r="F68" s="20"/>
       <c r="G68" s="3"/>
@@ -3366,20 +3371,20 @@
       <c r="T68" s="3"/>
     </row>
     <row r="69" spans="1:20" ht="42">
-      <c r="A69" s="47">
+      <c r="A69" s="43">
         <v>6.11</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D69" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D69" s="46" t="s">
         <v>41</v>
       </c>
       <c r="E69" s="34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F69" s="20"/>
       <c r="G69" s="3"/>
@@ -3398,14 +3403,14 @@
       <c r="T69" s="3"/>
     </row>
     <row r="70" spans="1:20" ht="14">
-      <c r="A70" s="48"/>
+      <c r="A70" s="44"/>
       <c r="B70" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D70" s="48"/>
+        <v>148</v>
+      </c>
+      <c r="D70" s="44"/>
       <c r="E70" s="35"/>
       <c r="F70" s="20"/>
       <c r="G70" s="3"/>
@@ -3424,20 +3429,20 @@
       <c r="T70" s="3"/>
     </row>
     <row r="71" spans="1:20" ht="56">
-      <c r="A71" s="47">
+      <c r="A71" s="43">
         <v>6.12</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D71" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="D71" s="46" t="s">
         <v>41</v>
       </c>
       <c r="E71" s="34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F71" s="20"/>
       <c r="G71" s="3"/>
@@ -3456,14 +3461,14 @@
       <c r="T71" s="3"/>
     </row>
     <row r="72" spans="1:20" ht="14">
-      <c r="A72" s="48"/>
+      <c r="A72" s="44"/>
       <c r="B72" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D72" s="48"/>
+        <v>152</v>
+      </c>
+      <c r="D72" s="44"/>
       <c r="E72" s="35"/>
       <c r="F72" s="20"/>
       <c r="G72" s="3"/>
@@ -3486,14 +3491,14 @@
         <v>6.13</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>68</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F73" s="27"/>
       <c r="G73" s="8"/>
@@ -3512,13 +3517,13 @@
       <c r="T73" s="3"/>
     </row>
     <row r="74" spans="1:20" ht="13">
-      <c r="A74" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B74" s="38"/>
-      <c r="C74" s="38"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="39"/>
+      <c r="A74" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="B74" s="41"/>
+      <c r="C74" s="41"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="42"/>
       <c r="F74" s="20"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
@@ -3536,10 +3541,10 @@
       <c r="T74" s="3"/>
     </row>
     <row r="75" spans="1:20" ht="13">
-      <c r="A75" s="42"/>
-      <c r="B75" s="43"/>
-      <c r="C75" s="43"/>
-      <c r="D75" s="44"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="38"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="39"/>
       <c r="E75" s="13"/>
       <c r="F75" s="20"/>
       <c r="G75" s="3"/>
@@ -3562,7 +3567,7 @@
         <v>6.14</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>68</v>
@@ -3571,7 +3576,7 @@
         <v>41</v>
       </c>
       <c r="E76" s="36" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F76" s="20"/>
       <c r="G76" s="8"/>
@@ -3594,14 +3599,14 @@
         <v>6.15</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F77" s="20"/>
       <c r="G77" s="3"/>
@@ -3621,16 +3626,16 @@
     </row>
     <row r="78" spans="1:20" ht="42">
       <c r="A78" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>10</v>
@@ -3656,7 +3661,7 @@
         <v>7.1</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>7</v>
@@ -3665,7 +3670,7 @@
         <v>8</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F79" s="20"/>
       <c r="G79" s="3"/>
@@ -21395,6 +21400,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A74:E74"/>
     <mergeCell ref="A75:D75"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A67:A68"/>
@@ -21403,21 +21423,6 @@
     <mergeCell ref="D69:D70"/>
     <mergeCell ref="A71:A72"/>
     <mergeCell ref="D71:D72"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A54:E54"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A74:E74"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="A9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>